<commit_message>
Menambahkan pengiriman notifikasi via telegram
</commit_message>
<xml_diff>
--- a/assets/excel/contoh.xlsx
+++ b/assets/excel/contoh.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nama</t>
   </si>
@@ -59,16 +59,25 @@
     <t>Haruka</t>
   </si>
   <si>
-    <t>089907212341</t>
-  </si>
-  <si>
-    <t>085156084242</t>
-  </si>
-  <si>
-    <t>082456084203</t>
-  </si>
-  <si>
     <t>haruna@gmail.com</t>
+  </si>
+  <si>
+    <t>Username Telegram</t>
+  </si>
+  <si>
+    <t>hodsiador</t>
+  </si>
+  <si>
+    <t>harugpa</t>
+  </si>
+  <si>
+    <t>+6289907212341</t>
+  </si>
+  <si>
+    <t>+6285156084242</t>
+  </si>
+  <si>
+    <t>+6282456084203</t>
   </si>
 </sst>
 </file>
@@ -432,69 +441,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" t="s">
         <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+  <ignoredErrors>
+    <ignoredError sqref="C4 C2:C3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>